<commit_message>
scores on 100 samples for all features
</commit_message>
<xml_diff>
--- a/training_features/2024-11-21_15-40-46/scores_llama3.1_8b_0-shot_100.xlsx
+++ b/training_features/2024-11-21_15-40-46/scores_llama3.1_8b_0-shot_100.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O45"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,70 +436,90 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>features</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>features</t>
+          <t>ridge-mse</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>ridge-mse</t>
+          <t>ridge-mae</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>ridge-mae</t>
+          <t>ridge-rmse</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>ridge-rmse</t>
+          <t>ridge-r2</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>ridge-r2</t>
+          <t>mse</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>mae</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>rmse</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>r2</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>xgboost-mse</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>xgboost-mae</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>xgboost-rmse</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>xgboost-r2</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>lasso-mse</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>lasso-mae</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>lasso-rmse</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>lasso-r2</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>num_datasets</t>
         </is>
@@ -509,74 +529,86 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>baseline-raw</t>
         </is>
       </c>
+      <c r="C2" t="n">
+        <v>2.26</v>
+      </c>
       <c r="D2" t="n">
-        <v>0.2563315001620023</v>
+        <v>1.34</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4146365466089677</v>
+        <v>1.5</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5062919120053196</v>
+        <v>0.47</v>
       </c>
       <c r="G2" t="n">
-        <v>0.05624829547031684</v>
+        <v>2.65</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>1.42</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1.63</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="K2" t="n">
-        <v>1.56881430347849</v>
+        <v>0.92</v>
       </c>
       <c r="L2" t="n">
-        <v>1.169872929519933</v>
+        <v>0.78</v>
       </c>
       <c r="M2" t="n">
-        <v>1.252523174826913</v>
+        <v>0.96</v>
       </c>
       <c r="N2" t="n">
-        <v>-4.776001669957251</v>
+        <v>0.78</v>
       </c>
       <c r="O2" t="n">
-        <v>3</v>
+        <v>2.28</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="S2" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>baseline-norm</t>
         </is>
       </c>
+      <c r="C3" t="n">
+        <v>0.01</v>
+      </c>
       <c r="D3" t="n">
-        <v>0.00159024629674011</v>
+        <v>0.1</v>
       </c>
       <c r="E3" t="n">
-        <v>0.03647289778796643</v>
+        <v>0.11</v>
       </c>
       <c r="F3" t="n">
-        <v>0.03987789233071514</v>
+        <v>0.59</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1732318747824875</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -585,47 +617,59 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>0.002426136622541559</v>
+        <v>0.01</v>
       </c>
       <c r="L3" t="n">
-        <v>0.03386970507747973</v>
+        <v>0.06</v>
       </c>
       <c r="M3" t="n">
-        <v>0.04925582831037927</v>
+        <v>0.08</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.2613470196736729</v>
+        <v>0.79</v>
       </c>
       <c r="O3" t="n">
-        <v>3</v>
+        <v>0.04</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="R3" t="n">
+        <v>-0.51</v>
+      </c>
+      <c r="S3" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>all-raw</t>
         </is>
       </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
       <c r="D4" t="n">
-        <v>0.1152139161393527</v>
+        <v>0.02</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3371900663275158</v>
+        <v>0.03</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3394317547598526</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9028492664506097</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -634,145 +678,181 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>0.4747313226773748</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="L4" t="n">
-        <v>0.6224190727518495</v>
+        <v>0.2</v>
       </c>
       <c r="M4" t="n">
-        <v>0.6890074910168792</v>
+        <v>0.27</v>
       </c>
       <c r="N4" t="n">
-        <v>0.5996968267166967</v>
+        <v>0.92</v>
       </c>
       <c r="O4" t="n">
-        <v>3</v>
+        <v>0.01</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="S4" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>all-norm</t>
         </is>
       </c>
+      <c r="C5" t="n">
+        <v>0.05</v>
+      </c>
       <c r="D5" t="n">
-        <v>0.02092874342054181</v>
+        <v>0.21</v>
       </c>
       <c r="E5" t="n">
-        <v>0.120454602429977</v>
+        <v>0.23</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1446676999905017</v>
+        <v>0.1</v>
       </c>
       <c r="G5" t="n">
-        <v>0.9030769339179566</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>0.22</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>0.27</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>-0.17</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1956501790012919</v>
+        <v>0.06</v>
       </c>
       <c r="L5" t="n">
-        <v>0.377899027074944</v>
+        <v>0.21</v>
       </c>
       <c r="M5" t="n">
-        <v>0.4423236134339788</v>
+        <v>0.25</v>
       </c>
       <c r="N5" t="n">
-        <v>0.09392480727278574</v>
+        <v>-0.04</v>
       </c>
       <c r="O5" t="n">
-        <v>3</v>
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="R5" t="n">
+        <v>-0.08</v>
+      </c>
+      <c r="S5" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>baseline-raw</t>
         </is>
       </c>
+      <c r="C6" t="n">
+        <v>1.04</v>
+      </c>
       <c r="D6" t="n">
-        <v>0.6651168805479737</v>
+        <v>0.87</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5745082830403663</v>
+        <v>1.02</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8155469824283416</v>
+        <v>0.26</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.03439599825698059</v>
+        <v>1.1</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>0.89</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1.05</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>0.22</v>
       </c>
       <c r="K6" t="n">
-        <v>0.6511419851565289</v>
+        <v>0.46</v>
       </c>
       <c r="L6" t="n">
-        <v>0.5663228208029769</v>
+        <v>0.57</v>
       </c>
       <c r="M6" t="n">
-        <v>0.806933693159809</v>
+        <v>0.68</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.0126621101363531</v>
+        <v>0.68</v>
       </c>
       <c r="O6" t="n">
-        <v>12</v>
+        <v>0.96</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="S6" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>baseline-norm</t>
         </is>
       </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
       <c r="D7" t="n">
-        <v>0.002342597799835311</v>
+        <v>0.04</v>
       </c>
       <c r="E7" t="n">
-        <v>0.03463759755415401</v>
+        <v>0.05</v>
       </c>
       <c r="F7" t="n">
-        <v>0.04840039049259118</v>
+        <v>0.89</v>
       </c>
       <c r="G7" t="n">
-        <v>0.8347335539895558</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -781,47 +861,59 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" t="n">
-        <v>0.01507554298262903</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>0.08882161353446709</v>
+        <v>0.04</v>
       </c>
       <c r="M7" t="n">
-        <v>0.1227825027543788</v>
+        <v>0.06</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.06355491778910882</v>
+        <v>0.85</v>
       </c>
       <c r="O7" t="n">
-        <v>12</v>
+        <v>0.02</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="S7" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B8" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>all-raw</t>
         </is>
       </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
       <c r="D8" t="n">
-        <v>0.0004737813098467893</v>
+        <v>0.03</v>
       </c>
       <c r="E8" t="n">
-        <v>0.01823133503111588</v>
+        <v>0.04</v>
       </c>
       <c r="F8" t="n">
-        <v>0.02176651809194087</v>
+        <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>0.9990745063028126</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -830,145 +922,181 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>0.06053905575154444</v>
+        <v>0.42</v>
       </c>
       <c r="L8" t="n">
-        <v>0.2105911472868759</v>
+        <v>0.47</v>
       </c>
       <c r="M8" t="n">
-        <v>0.2460468568211032</v>
+        <v>0.65</v>
       </c>
       <c r="N8" t="n">
-        <v>0.8817418218759022</v>
+        <v>0.61</v>
       </c>
       <c r="O8" t="n">
-        <v>12</v>
+        <v>0.02</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="S8" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B9" t="n">
-        <v>3</v>
-      </c>
-      <c r="C9" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>all-norm</t>
         </is>
       </c>
+      <c r="C9" t="n">
+        <v>0.03</v>
+      </c>
       <c r="D9" t="n">
-        <v>0.02148291095491551</v>
+        <v>0.14</v>
       </c>
       <c r="E9" t="n">
-        <v>0.104328537766621</v>
+        <v>0.17</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1465704982420252</v>
+        <v>0.49</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4223469506693399</v>
+        <v>0.75</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>0.49</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>0.87</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>-12.39</v>
       </c>
       <c r="K9" t="n">
-        <v>0.03680001488826504</v>
+        <v>0.03</v>
       </c>
       <c r="L9" t="n">
-        <v>0.1458826275202691</v>
+        <v>0.09</v>
       </c>
       <c r="M9" t="n">
-        <v>0.1918332997377281</v>
+        <v>0.19</v>
       </c>
       <c r="N9" t="n">
-        <v>0.01048601559482676</v>
+        <v>0.38</v>
       </c>
       <c r="O9" t="n">
-        <v>12</v>
+        <v>0.05</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="S9" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>baseline-raw</t>
         </is>
       </c>
+      <c r="C10" t="n">
+        <v>0.43</v>
+      </c>
       <c r="D10" t="n">
-        <v>2.743009508003611</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="E10" t="n">
-        <v>1.442868156939601</v>
+        <v>0.65</v>
       </c>
       <c r="F10" t="n">
-        <v>1.65620334138161</v>
+        <v>0.71</v>
       </c>
       <c r="G10" t="n">
-        <v>-1.731328101517981</v>
+        <v>0.47</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>0.57</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>0.68</v>
       </c>
       <c r="K10" t="n">
-        <v>2.342404610947153</v>
+        <v>0.23</v>
       </c>
       <c r="L10" t="n">
-        <v>1.318411503165864</v>
+        <v>0.32</v>
       </c>
       <c r="M10" t="n">
-        <v>1.530491623938907</v>
+        <v>0.48</v>
       </c>
       <c r="N10" t="n">
-        <v>-1.332429224301774</v>
+        <v>0.84</v>
       </c>
       <c r="O10" t="n">
-        <v>4</v>
+        <v>0.48</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="S10" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>baseline-norm</t>
         </is>
       </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
       <c r="D11" t="n">
-        <v>0.002373924901880895</v>
+        <v>0.04</v>
       </c>
       <c r="E11" t="n">
-        <v>0.04435668901361192</v>
+        <v>0.05</v>
       </c>
       <c r="F11" t="n">
-        <v>0.04872294020152002</v>
+        <v>0.8</v>
       </c>
       <c r="G11" t="n">
-        <v>0.4962556143935565</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -977,47 +1105,59 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" t="n">
-        <v>0.004248026376519386</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>0.05155475597127121</v>
+        <v>0.04</v>
       </c>
       <c r="M11" t="n">
-        <v>0.06517688529317266</v>
+        <v>0.05</v>
       </c>
       <c r="N11" t="n">
-        <v>0.09857323819121844</v>
+        <v>0.79</v>
       </c>
       <c r="O11" t="n">
-        <v>4</v>
+        <v>0.01</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="S11" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B12" t="n">
-        <v>2</v>
-      </c>
-      <c r="C12" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>all-raw</t>
         </is>
       </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
       <c r="D12" t="n">
-        <v>0.05136501158738765</v>
+        <v>0.02</v>
       </c>
       <c r="E12" t="n">
-        <v>0.2125376219870391</v>
+        <v>0.03</v>
       </c>
       <c r="F12" t="n">
-        <v>0.2266385042030318</v>
+        <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.4121428817566626</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1026,145 +1166,181 @@
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" t="n">
-        <v>0.04583328506000877</v>
+        <v>0.08</v>
       </c>
       <c r="L12" t="n">
-        <v>0.1980819256357898</v>
+        <v>0.22</v>
       </c>
       <c r="M12" t="n">
-        <v>0.2140870969021925</v>
+        <v>0.27</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.2600629347644834</v>
+        <v>0.89</v>
       </c>
       <c r="O12" t="n">
-        <v>4</v>
+        <v>0.02</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="S12" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B13" t="n">
-        <v>3</v>
-      </c>
-      <c r="C13" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>all-norm</t>
         </is>
       </c>
+      <c r="C13" t="n">
+        <v>0.03</v>
+      </c>
       <c r="D13" t="n">
-        <v>0.1017647014879261</v>
+        <v>0.16</v>
       </c>
       <c r="E13" t="n">
-        <v>0.2901611745943962</v>
+        <v>0.18</v>
       </c>
       <c r="F13" t="n">
-        <v>0.319005801652456</v>
+        <v>0.31</v>
       </c>
       <c r="G13" t="n">
-        <v>0.5473308202315349</v>
+        <v>0.03</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>0.48</v>
       </c>
       <c r="K13" t="n">
-        <v>0.206077497933531</v>
+        <v>0.02</v>
       </c>
       <c r="L13" t="n">
-        <v>0.3988708179065623</v>
+        <v>0.11</v>
       </c>
       <c r="M13" t="n">
-        <v>0.4539575948627041</v>
+        <v>0.15</v>
       </c>
       <c r="N13" t="n">
-        <v>0.0833272186291738</v>
+        <v>0.53</v>
       </c>
       <c r="O13" t="n">
-        <v>4</v>
+        <v>0.06</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="R13" t="n">
+        <v>-0.19</v>
+      </c>
+      <c r="S13" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>baseline-raw</t>
         </is>
       </c>
+      <c r="C14" t="n">
+        <v>0.54</v>
+      </c>
       <c r="D14" t="n">
-        <v>4.134589132452867</v>
+        <v>0.61</v>
       </c>
       <c r="E14" t="n">
-        <v>1.831523226911435</v>
+        <v>0.74</v>
       </c>
       <c r="F14" t="n">
-        <v>2.033368912040525</v>
+        <v>0.38</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.1737857068417328</v>
+        <v>0.63</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>0.64</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>0.79</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>0.28</v>
       </c>
       <c r="K14" t="n">
-        <v>3.789032027998909</v>
+        <v>0.25</v>
       </c>
       <c r="L14" t="n">
-        <v>1.799523338047448</v>
+        <v>0.38</v>
       </c>
       <c r="M14" t="n">
-        <v>1.946543610608021</v>
+        <v>0.5</v>
       </c>
       <c r="N14" t="n">
-        <v>-0.07568406309628961</v>
+        <v>0.72</v>
       </c>
       <c r="O14" t="n">
-        <v>5</v>
+        <v>0.5</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="S14" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>baseline-norm</t>
         </is>
       </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
       <c r="D15" t="n">
-        <v>0.005030582669058531</v>
+        <v>0.05</v>
       </c>
       <c r="E15" t="n">
-        <v>0.05199202100929382</v>
+        <v>0.06</v>
       </c>
       <c r="F15" t="n">
-        <v>0.07092660057452727</v>
+        <v>0.88</v>
       </c>
       <c r="G15" t="n">
-        <v>0.7934116464805459</v>
+        <v>0</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1173,47 +1349,59 @@
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" t="n">
-        <v>0.02435980696033527</v>
+        <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>0.1157207759470003</v>
+        <v>0.04</v>
       </c>
       <c r="M15" t="n">
-        <v>0.1560762857077758</v>
+        <v>0.05</v>
       </c>
       <c r="N15" t="n">
-        <v>-0.0003716752217137742</v>
+        <v>0.92</v>
       </c>
       <c r="O15" t="n">
-        <v>5</v>
+        <v>0.03</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="R15" t="n">
+        <v>-0.04</v>
+      </c>
+      <c r="S15" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B16" t="n">
-        <v>2</v>
-      </c>
-      <c r="C16" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>all-raw</t>
         </is>
       </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
       <c r="D16" t="n">
-        <v>0.003862972518297138</v>
+        <v>0.01</v>
       </c>
       <c r="E16" t="n">
-        <v>0.04635445252120215</v>
+        <v>0.02</v>
       </c>
       <c r="F16" t="n">
-        <v>0.06215281585171454</v>
+        <v>1</v>
       </c>
       <c r="G16" t="n">
-        <v>0.9954521003844352</v>
+        <v>0</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1222,145 +1410,181 @@
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16" t="n">
-        <v>0.03183450562622359</v>
+        <v>0.04</v>
       </c>
       <c r="L16" t="n">
-        <v>0.1667057272883887</v>
+        <v>0.17</v>
       </c>
       <c r="M16" t="n">
-        <v>0.1784222677420719</v>
+        <v>0.19</v>
       </c>
       <c r="N16" t="n">
-        <v>0.9625210546506762</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="O16" t="n">
-        <v>5</v>
+        <v>0.01</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="S16" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B17" t="n">
-        <v>3</v>
-      </c>
-      <c r="C17" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>all-norm</t>
         </is>
       </c>
+      <c r="C17" t="n">
+        <v>0.02</v>
+      </c>
       <c r="D17" t="n">
-        <v>0.1132051150017935</v>
+        <v>0.11</v>
       </c>
       <c r="E17" t="n">
-        <v>0.3241280928082168</v>
+        <v>0.14</v>
       </c>
       <c r="F17" t="n">
-        <v>0.3364596781217528</v>
+        <v>0.24</v>
       </c>
       <c r="G17" t="n">
-        <v>-1.268731589209038</v>
+        <v>0.02</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="K17" t="n">
-        <v>0.16059654407255</v>
+        <v>0.02</v>
       </c>
       <c r="L17" t="n">
-        <v>0.3435587880404756</v>
+        <v>0.09</v>
       </c>
       <c r="M17" t="n">
-        <v>0.4007449863348885</v>
+        <v>0.13</v>
       </c>
       <c r="N17" t="n">
-        <v>-2.218498145153807</v>
+        <v>0.41</v>
       </c>
       <c r="O17" t="n">
-        <v>5</v>
+        <v>0.03</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="R17" t="n">
+        <v>-0.09</v>
+      </c>
+      <c r="S17" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B18" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" t="inlineStr">
+      <c r="B18" t="inlineStr">
         <is>
           <t>baseline-raw</t>
         </is>
       </c>
+      <c r="C18" t="n">
+        <v>0.45</v>
+      </c>
       <c r="D18" t="n">
-        <v>1.418412304569241</v>
+        <v>0.49</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9901159075665164</v>
+        <v>0.67</v>
       </c>
       <c r="F18" t="n">
-        <v>1.19097116025924</v>
+        <v>0.7</v>
       </c>
       <c r="G18" t="n">
-        <v>-1.916048597160791</v>
+        <v>0.46</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>0.49</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>0.68</v>
       </c>
       <c r="J18" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="K18" t="n">
-        <v>1.126368874639605</v>
+        <v>0.29</v>
       </c>
       <c r="L18" t="n">
-        <v>0.8674679252199087</v>
+        <v>0.38</v>
       </c>
       <c r="M18" t="n">
-        <v>1.061305269297955</v>
+        <v>0.54</v>
       </c>
       <c r="N18" t="n">
-        <v>-1.31564994620932</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="O18" t="n">
-        <v>6</v>
+        <v>0.48</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="S18" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" t="inlineStr">
+      <c r="B19" t="inlineStr">
         <is>
           <t>baseline-norm</t>
         </is>
       </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
       <c r="D19" t="n">
-        <v>0.007406960617049317</v>
+        <v>0.04</v>
       </c>
       <c r="E19" t="n">
-        <v>0.07603749834942523</v>
+        <v>0.05</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0860637009258219</v>
+        <v>0.9</v>
       </c>
       <c r="G19" t="n">
-        <v>0.6468949389758432</v>
+        <v>0</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -1369,47 +1593,59 @@
         <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" t="n">
-        <v>0.02704214331241875</v>
+        <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>0.1231842418601109</v>
+        <v>0.03</v>
       </c>
       <c r="M19" t="n">
-        <v>0.1644449552659453</v>
+        <v>0.04</v>
       </c>
       <c r="N19" t="n">
-        <v>-0.2891546422666824</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="O19" t="n">
-        <v>6</v>
+        <v>0.03</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B20" t="n">
-        <v>2</v>
-      </c>
-      <c r="C20" t="inlineStr">
+      <c r="B20" t="inlineStr">
         <is>
           <t>all-raw</t>
         </is>
       </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
       <c r="D20" t="n">
-        <v>0.005144474846533874</v>
+        <v>0.01</v>
       </c>
       <c r="E20" t="n">
-        <v>0.06156198088681532</v>
+        <v>0.01</v>
       </c>
       <c r="F20" t="n">
-        <v>0.07172499457325789</v>
+        <v>1</v>
       </c>
       <c r="G20" t="n">
-        <v>0.9945572059393775</v>
+        <v>0</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
@@ -1418,145 +1654,181 @@
         <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" t="n">
-        <v>0.0823899937355759</v>
+        <v>0.04</v>
       </c>
       <c r="L20" t="n">
-        <v>0.2476485450171625</v>
+        <v>0.12</v>
       </c>
       <c r="M20" t="n">
-        <v>0.2870365721220484</v>
+        <v>0.19</v>
       </c>
       <c r="N20" t="n">
-        <v>0.9128323527792436</v>
+        <v>0.93</v>
       </c>
       <c r="O20" t="n">
-        <v>6</v>
+        <v>0.01</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="S20" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B21" t="n">
-        <v>3</v>
-      </c>
-      <c r="C21" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>all-norm</t>
         </is>
       </c>
+      <c r="C21" t="n">
+        <v>0.03</v>
+      </c>
       <c r="D21" t="n">
-        <v>0.0551339194698582</v>
+        <v>0.13</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1970933903688751</v>
+        <v>0.16</v>
       </c>
       <c r="F21" t="n">
-        <v>0.2348061316700614</v>
+        <v>0.38</v>
       </c>
       <c r="G21" t="n">
-        <v>0.3920460623742131</v>
+        <v>0.02</v>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>0.42</v>
       </c>
       <c r="K21" t="n">
-        <v>0.0988458281244297</v>
+        <v>0.01</v>
       </c>
       <c r="L21" t="n">
-        <v>0.259822169968092</v>
+        <v>0.06</v>
       </c>
       <c r="M21" t="n">
-        <v>0.3143975638016772</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="N21" t="n">
-        <v>-0.0899589763245856</v>
+        <v>0.88</v>
       </c>
       <c r="O21" t="n">
-        <v>6</v>
+        <v>0.04</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="S21" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B22" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" t="inlineStr">
+      <c r="B22" t="inlineStr">
         <is>
           <t>baseline-raw</t>
         </is>
       </c>
+      <c r="C22" t="n">
+        <v>0.91</v>
+      </c>
       <c r="D22" t="n">
-        <v>0.988713739268878</v>
+        <v>0.8</v>
       </c>
       <c r="E22" t="n">
-        <v>0.9016766539580833</v>
+        <v>0.95</v>
       </c>
       <c r="F22" t="n">
-        <v>0.9943408566828972</v>
+        <v>0.37</v>
       </c>
       <c r="G22" t="n">
-        <v>0.2431850909452904</v>
+        <v>0.93</v>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>0.96</v>
       </c>
       <c r="J22" t="n">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="K22" t="n">
-        <v>0.8567999450723214</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="L22" t="n">
-        <v>0.8571487478823986</v>
+        <v>0.2</v>
       </c>
       <c r="M22" t="n">
-        <v>0.9256348875622188</v>
+        <v>0.27</v>
       </c>
       <c r="N22" t="n">
-        <v>0.3441590353670124</v>
+        <v>0.95</v>
       </c>
       <c r="O22" t="n">
-        <v>7</v>
+        <v>0.87</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="S22" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B23" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" t="inlineStr">
+      <c r="B23" t="inlineStr">
         <is>
           <t>baseline-norm</t>
         </is>
       </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
       <c r="D23" t="n">
-        <v>0.01071113306760942</v>
+        <v>0.04</v>
       </c>
       <c r="E23" t="n">
-        <v>0.09449068789923874</v>
+        <v>0.04</v>
       </c>
       <c r="F23" t="n">
-        <v>0.1034946040506916</v>
+        <v>0.9</v>
       </c>
       <c r="G23" t="n">
-        <v>0.6829562091896402</v>
+        <v>0</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -1565,47 +1837,59 @@
         <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" t="n">
-        <v>0.04058982472752849</v>
+        <v>0</v>
       </c>
       <c r="L23" t="n">
-        <v>0.1712136877267833</v>
+        <v>0.02</v>
       </c>
       <c r="M23" t="n">
-        <v>0.201469165699192</v>
+        <v>0.03</v>
       </c>
       <c r="N23" t="n">
-        <v>-0.2014370299309374</v>
+        <v>0.95</v>
       </c>
       <c r="O23" t="n">
-        <v>7</v>
+        <v>0.02</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R23" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="S23" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B24" t="n">
-        <v>2</v>
-      </c>
-      <c r="C24" t="inlineStr">
+      <c r="B24" t="inlineStr">
         <is>
           <t>all-raw</t>
         </is>
       </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
       <c r="D24" t="n">
-        <v>0.004244403261291197</v>
+        <v>0.01</v>
       </c>
       <c r="E24" t="n">
-        <v>0.05597155492351879</v>
+        <v>0.01</v>
       </c>
       <c r="F24" t="n">
-        <v>0.06514908488452617</v>
+        <v>1</v>
       </c>
       <c r="G24" t="n">
-        <v>0.9939491152110917</v>
+        <v>0</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -1614,145 +1898,181 @@
         <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" t="n">
-        <v>0.03638463794564235</v>
+        <v>0.04</v>
       </c>
       <c r="L24" t="n">
-        <v>0.1631729047094838</v>
+        <v>0.13</v>
       </c>
       <c r="M24" t="n">
-        <v>0.1907475765131561</v>
+        <v>0.19</v>
       </c>
       <c r="N24" t="n">
-        <v>0.9481295158018876</v>
+        <v>0.93</v>
       </c>
       <c r="O24" t="n">
-        <v>7</v>
+        <v>0.01</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="S24" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B25" t="n">
-        <v>3</v>
-      </c>
-      <c r="C25" t="inlineStr">
+      <c r="B25" t="inlineStr">
         <is>
           <t>all-norm</t>
         </is>
       </c>
+      <c r="C25" t="n">
+        <v>0.02</v>
+      </c>
       <c r="D25" t="n">
-        <v>0.0538158183114108</v>
+        <v>0.1</v>
       </c>
       <c r="E25" t="n">
-        <v>0.2147776515832861</v>
+        <v>0.14</v>
       </c>
       <c r="F25" t="n">
-        <v>0.2319823663803152</v>
+        <v>0.44</v>
       </c>
       <c r="G25" t="n">
-        <v>0.2648572857296065</v>
+        <v>0.01</v>
       </c>
       <c r="H25" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="J25" t="n">
-        <v>0</v>
+        <v>0.55</v>
       </c>
       <c r="K25" t="n">
-        <v>0.0815301878709216</v>
+        <v>0.02</v>
       </c>
       <c r="L25" t="n">
-        <v>0.2266406501227361</v>
+        <v>0.08</v>
       </c>
       <c r="M25" t="n">
-        <v>0.2855349153272181</v>
+        <v>0.15</v>
       </c>
       <c r="N25" t="n">
-        <v>-0.1137305997945934</v>
+        <v>0.34</v>
       </c>
       <c r="O25" t="n">
-        <v>7</v>
+        <v>0.03</v>
+      </c>
+      <c r="P25" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="S25" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B26" t="n">
-        <v>0</v>
-      </c>
-      <c r="C26" t="inlineStr">
+      <c r="B26" t="inlineStr">
         <is>
           <t>baseline-raw</t>
         </is>
       </c>
+      <c r="C26" t="n">
+        <v>0.76</v>
+      </c>
       <c r="D26" t="n">
-        <v>1.292963853778752</v>
+        <v>0.68</v>
       </c>
       <c r="E26" t="n">
-        <v>0.9055804118682681</v>
+        <v>0.87</v>
       </c>
       <c r="F26" t="n">
-        <v>1.137085684448957</v>
+        <v>0.53</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.6901272370970439</v>
+        <v>0.77</v>
       </c>
       <c r="H26" t="n">
-        <v>0</v>
+        <v>0.68</v>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>0.88</v>
       </c>
       <c r="J26" t="n">
-        <v>0</v>
+        <v>0.52</v>
       </c>
       <c r="K26" t="n">
-        <v>1.037206616128021</v>
+        <v>0.3</v>
       </c>
       <c r="L26" t="n">
-        <v>0.8837372574145544</v>
+        <v>0.33</v>
       </c>
       <c r="M26" t="n">
-        <v>1.018433412711907</v>
+        <v>0.55</v>
       </c>
       <c r="N26" t="n">
-        <v>-0.3558083215489452</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="O26" t="n">
-        <v>8</v>
+        <v>0.77</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="S26" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B27" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" t="inlineStr">
+      <c r="B27" t="inlineStr">
         <is>
           <t>baseline-norm</t>
         </is>
       </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
       <c r="D27" t="n">
-        <v>0.003835376880421413</v>
+        <v>0.02</v>
       </c>
       <c r="E27" t="n">
-        <v>0.04136122683413001</v>
+        <v>0.03</v>
       </c>
       <c r="F27" t="n">
-        <v>0.06193041966934677</v>
+        <v>0.93</v>
       </c>
       <c r="G27" t="n">
-        <v>0.8478791820777187</v>
+        <v>0</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
@@ -1761,47 +2081,59 @@
         <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" t="n">
-        <v>0.02809918013132333</v>
+        <v>0</v>
       </c>
       <c r="L27" t="n">
-        <v>0.1228892159781628</v>
+        <v>0.03</v>
       </c>
       <c r="M27" t="n">
-        <v>0.1676281006613251</v>
+        <v>0.04</v>
       </c>
       <c r="N27" t="n">
-        <v>-0.1144850682973202</v>
+        <v>0.9</v>
       </c>
       <c r="O27" t="n">
-        <v>8</v>
+        <v>0.02</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="R27" t="n">
+        <v>-0</v>
+      </c>
+      <c r="S27" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B28" t="n">
-        <v>2</v>
-      </c>
-      <c r="C28" t="inlineStr">
+      <c r="B28" t="inlineStr">
         <is>
           <t>all-raw</t>
         </is>
       </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
       <c r="D28" t="n">
-        <v>0.004999883824281021</v>
+        <v>0.01</v>
       </c>
       <c r="E28" t="n">
-        <v>0.06064182018415945</v>
+        <v>0.01</v>
       </c>
       <c r="F28" t="n">
-        <v>0.07070985662749586</v>
+        <v>1</v>
       </c>
       <c r="G28" t="n">
-        <v>0.9861657175692256</v>
+        <v>0</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
@@ -1810,145 +2142,181 @@
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" t="n">
-        <v>0.0698997124504568</v>
+        <v>0.03</v>
       </c>
       <c r="L28" t="n">
-        <v>0.2309332804998625</v>
+        <v>0.13</v>
       </c>
       <c r="M28" t="n">
-        <v>0.2643855375213569</v>
+        <v>0.17</v>
       </c>
       <c r="N28" t="n">
-        <v>0.8065930333874122</v>
+        <v>0.96</v>
       </c>
       <c r="O28" t="n">
-        <v>8</v>
+        <v>0.01</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="S28" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B29" t="n">
-        <v>3</v>
-      </c>
-      <c r="C29" t="inlineStr">
+      <c r="B29" t="inlineStr">
         <is>
           <t>all-norm</t>
         </is>
       </c>
+      <c r="C29" t="n">
+        <v>0.02</v>
+      </c>
       <c r="D29" t="n">
-        <v>0.0236240382905077</v>
+        <v>0.1</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1342551884699202</v>
+        <v>0.14</v>
       </c>
       <c r="F29" t="n">
-        <v>0.1537011330163434</v>
+        <v>0.59</v>
       </c>
       <c r="G29" t="n">
-        <v>0.1634120063932867</v>
+        <v>0.02</v>
       </c>
       <c r="H29" t="n">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="I29" t="n">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="J29" t="n">
-        <v>0</v>
+        <v>0.68</v>
       </c>
       <c r="K29" t="n">
-        <v>0.03776709644250763</v>
+        <v>0.01</v>
       </c>
       <c r="L29" t="n">
-        <v>0.1365855270378441</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="M29" t="n">
-        <v>0.1943375837106854</v>
+        <v>0.1</v>
       </c>
       <c r="N29" t="n">
-        <v>-0.3374300806938664</v>
+        <v>0.8</v>
       </c>
       <c r="O29" t="n">
-        <v>8</v>
+        <v>0.05</v>
+      </c>
+      <c r="P29" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="R29" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="S29" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B30" t="n">
-        <v>0</v>
-      </c>
-      <c r="C30" t="inlineStr">
+      <c r="B30" t="inlineStr">
         <is>
           <t>baseline-raw</t>
         </is>
       </c>
+      <c r="C30" t="n">
+        <v>0.89</v>
+      </c>
       <c r="D30" t="n">
-        <v>1.312546458388968</v>
+        <v>0.71</v>
       </c>
       <c r="E30" t="n">
-        <v>0.8955663728695225</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="F30" t="n">
-        <v>1.145664199662784</v>
+        <v>0.47</v>
       </c>
       <c r="G30" t="n">
-        <v>0.06804099051130386</v>
+        <v>0.92</v>
       </c>
       <c r="H30" t="n">
-        <v>0</v>
+        <v>0.73</v>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>0.96</v>
       </c>
       <c r="J30" t="n">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="K30" t="n">
-        <v>1.256140915138356</v>
+        <v>0.14</v>
       </c>
       <c r="L30" t="n">
-        <v>0.8818894117720616</v>
+        <v>0.28</v>
       </c>
       <c r="M30" t="n">
-        <v>1.120776924788495</v>
+        <v>0.37</v>
       </c>
       <c r="N30" t="n">
-        <v>0.1080911189326891</v>
+        <v>0.92</v>
       </c>
       <c r="O30" t="n">
-        <v>9</v>
+        <v>0.86</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="S30" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B31" t="n">
-        <v>1</v>
-      </c>
-      <c r="C31" t="inlineStr">
+      <c r="B31" t="inlineStr">
         <is>
           <t>baseline-norm</t>
         </is>
       </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
       <c r="D31" t="n">
-        <v>0.002673213705228096</v>
+        <v>0.03</v>
       </c>
       <c r="E31" t="n">
-        <v>0.03959232182809783</v>
+        <v>0.03</v>
       </c>
       <c r="F31" t="n">
-        <v>0.05170313051671142</v>
+        <v>0.91</v>
       </c>
       <c r="G31" t="n">
-        <v>0.8451194345182609</v>
+        <v>0</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -1957,47 +2325,59 @@
         <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31" t="n">
-        <v>0.02293591309537023</v>
+        <v>0</v>
       </c>
       <c r="L31" t="n">
-        <v>0.1173218133621848</v>
+        <v>0.03</v>
       </c>
       <c r="M31" t="n">
-        <v>0.1514460732253241</v>
+        <v>0.04</v>
       </c>
       <c r="N31" t="n">
-        <v>-0.3288601592545928</v>
+        <v>0.87</v>
       </c>
       <c r="O31" t="n">
-        <v>9</v>
+        <v>0.01</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0</v>
+      </c>
+      <c r="S31" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B32" t="n">
-        <v>2</v>
-      </c>
-      <c r="C32" t="inlineStr">
+      <c r="B32" t="inlineStr">
         <is>
           <t>all-raw</t>
         </is>
       </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
       <c r="D32" t="n">
-        <v>0.001051591662375078</v>
+        <v>0.01</v>
       </c>
       <c r="E32" t="n">
-        <v>0.02513372362102137</v>
+        <v>0.01</v>
       </c>
       <c r="F32" t="n">
-        <v>0.0324282540753442</v>
+        <v>1</v>
       </c>
       <c r="G32" t="n">
-        <v>0.9986489156072076</v>
+        <v>0</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -2006,658 +2386,94 @@
         <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K32" t="n">
-        <v>0.05253468654338588</v>
+        <v>0.02</v>
       </c>
       <c r="L32" t="n">
-        <v>0.1781430990902687</v>
+        <v>0.11</v>
       </c>
       <c r="M32" t="n">
-        <v>0.2292044644927011</v>
+        <v>0.15</v>
       </c>
       <c r="N32" t="n">
-        <v>0.9325034634558628</v>
+        <v>0.95</v>
       </c>
       <c r="O32" t="n">
-        <v>9</v>
+        <v>0.01</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="S32" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B33" t="n">
-        <v>3</v>
-      </c>
-      <c r="C33" t="inlineStr">
+      <c r="B33" t="inlineStr">
         <is>
           <t>all-norm</t>
         </is>
       </c>
+      <c r="C33" t="n">
+        <v>0.02</v>
+      </c>
       <c r="D33" t="n">
-        <v>0.03440152360921338</v>
+        <v>0.1</v>
       </c>
       <c r="E33" t="n">
-        <v>0.1526312286107874</v>
+        <v>0.13</v>
       </c>
       <c r="F33" t="n">
-        <v>0.1854764772396041</v>
+        <v>0.28</v>
       </c>
       <c r="G33" t="n">
-        <v>0.2774602987013874</v>
+        <v>0.02</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I33" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="J33" t="n">
-        <v>0</v>
+        <v>0.23</v>
       </c>
       <c r="K33" t="n">
-        <v>0.05955263488588128</v>
+        <v>0</v>
       </c>
       <c r="L33" t="n">
-        <v>0.1961744076718274</v>
+        <v>0.05</v>
       </c>
       <c r="M33" t="n">
-        <v>0.2440340855001229</v>
+        <v>0.06</v>
       </c>
       <c r="N33" t="n">
-        <v>-0.250791782096127</v>
+        <v>0.83</v>
       </c>
       <c r="O33" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B34" t="n">
-        <v>0</v>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>baseline-raw</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
-        <v>0.4800496808880096</v>
-      </c>
-      <c r="E34" t="n">
-        <v>0.5280274250586555</v>
-      </c>
-      <c r="F34" t="n">
-        <v>0.6928561761924401</v>
-      </c>
-      <c r="G34" t="n">
-        <v>0.543922360178595</v>
-      </c>
-      <c r="H34" t="n">
-        <v>0</v>
-      </c>
-      <c r="I34" t="n">
-        <v>0</v>
-      </c>
-      <c r="J34" t="n">
-        <v>0</v>
-      </c>
-      <c r="K34" t="n">
-        <v>0.4957350496976329</v>
-      </c>
-      <c r="L34" t="n">
-        <v>0.5287625125820319</v>
-      </c>
-      <c r="M34" t="n">
-        <v>0.7040845472651938</v>
-      </c>
-      <c r="N34" t="n">
-        <v>0.5290202651012939</v>
-      </c>
-      <c r="O34" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B35" t="n">
-        <v>1</v>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>baseline-norm</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
-        <v>0.004279370641382916</v>
-      </c>
-      <c r="E35" t="n">
-        <v>0.05068558113719699</v>
-      </c>
-      <c r="F35" t="n">
-        <v>0.06541689874476561</v>
-      </c>
-      <c r="G35" t="n">
-        <v>0.8313881066504163</v>
-      </c>
-      <c r="H35" t="n">
-        <v>0</v>
-      </c>
-      <c r="I35" t="n">
-        <v>0</v>
-      </c>
-      <c r="J35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K35" t="n">
-        <v>0.02641134720201314</v>
-      </c>
-      <c r="L35" t="n">
-        <v>0.1318995056127641</v>
-      </c>
-      <c r="M35" t="n">
-        <v>0.1625156829417184</v>
-      </c>
-      <c r="N35" t="n">
-        <v>-0.04063602591000537</v>
-      </c>
-      <c r="O35" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B36" t="n">
-        <v>2</v>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>all-raw</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
-        <v>0.0007738656154084155</v>
-      </c>
-      <c r="E36" t="n">
-        <v>0.02369470132871502</v>
-      </c>
-      <c r="F36" t="n">
-        <v>0.0278184402044474</v>
-      </c>
-      <c r="G36" t="n">
-        <v>0.9988383292025403</v>
-      </c>
-      <c r="H36" t="n">
-        <v>0</v>
-      </c>
-      <c r="I36" t="n">
-        <v>0</v>
-      </c>
-      <c r="J36" t="n">
-        <v>0</v>
-      </c>
-      <c r="K36" t="n">
-        <v>0.0619113898035307</v>
-      </c>
-      <c r="L36" t="n">
-        <v>0.2077558661849636</v>
-      </c>
-      <c r="M36" t="n">
-        <v>0.2488199947824344</v>
-      </c>
-      <c r="N36" t="n">
-        <v>0.9070631229338886</v>
-      </c>
-      <c r="O36" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B37" t="n">
-        <v>3</v>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>all-norm</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
-        <v>0.03494380181676177</v>
-      </c>
-      <c r="E37" t="n">
-        <v>0.1549402297848863</v>
-      </c>
-      <c r="F37" t="n">
-        <v>0.1869326130367887</v>
-      </c>
-      <c r="G37" t="n">
-        <v>0.1572863562260429</v>
-      </c>
-      <c r="H37" t="n">
-        <v>0</v>
-      </c>
-      <c r="I37" t="n">
-        <v>0</v>
-      </c>
-      <c r="J37" t="n">
-        <v>0</v>
-      </c>
-      <c r="K37" t="n">
-        <v>0.0452099444771262</v>
-      </c>
-      <c r="L37" t="n">
-        <v>0.1694876672356727</v>
-      </c>
-      <c r="M37" t="n">
-        <v>0.2126263024113579</v>
-      </c>
-      <c r="N37" t="n">
-        <v>-0.09029456053239282</v>
-      </c>
-      <c r="O37" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B38" t="n">
-        <v>0</v>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>baseline-raw</t>
-        </is>
-      </c>
-      <c r="D38" t="n">
-        <v>1.026925026771215</v>
-      </c>
-      <c r="E38" t="n">
-        <v>0.7792487785176159</v>
-      </c>
-      <c r="F38" t="n">
-        <v>1.013373093569794</v>
-      </c>
-      <c r="G38" t="n">
-        <v>0.2736841731108771</v>
-      </c>
-      <c r="H38" t="n">
-        <v>0</v>
-      </c>
-      <c r="I38" t="n">
-        <v>0</v>
-      </c>
-      <c r="J38" t="n">
-        <v>0</v>
-      </c>
-      <c r="K38" t="n">
-        <v>1.032612665801136</v>
-      </c>
-      <c r="L38" t="n">
-        <v>0.7728258631065714</v>
-      </c>
-      <c r="M38" t="n">
-        <v>1.016175509349215</v>
-      </c>
-      <c r="N38" t="n">
-        <v>0.2696614624578395</v>
-      </c>
-      <c r="O38" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B39" t="n">
-        <v>1</v>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>baseline-norm</t>
-        </is>
-      </c>
-      <c r="D39" t="n">
-        <v>0.001405359738042686</v>
-      </c>
-      <c r="E39" t="n">
-        <v>0.02693104668314261</v>
-      </c>
-      <c r="F39" t="n">
-        <v>0.03748812796129844</v>
-      </c>
-      <c r="G39" t="n">
-        <v>0.8606897681030241</v>
-      </c>
-      <c r="H39" t="n">
-        <v>0</v>
-      </c>
-      <c r="I39" t="n">
-        <v>0</v>
-      </c>
-      <c r="J39" t="n">
-        <v>0</v>
-      </c>
-      <c r="K39" t="n">
-        <v>0.01134989345307584</v>
-      </c>
-      <c r="L39" t="n">
-        <v>0.0829786774910969</v>
-      </c>
-      <c r="M39" t="n">
-        <v>0.1065358787126471</v>
-      </c>
-      <c r="N39" t="n">
-        <v>-0.1250900720666146</v>
-      </c>
-      <c r="O39" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B40" t="n">
-        <v>2</v>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>all-raw</t>
-        </is>
-      </c>
-      <c r="D40" t="n">
-        <v>0.0006631999104758697</v>
-      </c>
-      <c r="E40" t="n">
-        <v>0.02010327749835614</v>
-      </c>
-      <c r="F40" t="n">
-        <v>0.02575266802635932</v>
-      </c>
-      <c r="G40" t="n">
-        <v>0.998972839148087</v>
-      </c>
-      <c r="H40" t="n">
-        <v>0</v>
-      </c>
-      <c r="I40" t="n">
-        <v>0</v>
-      </c>
-      <c r="J40" t="n">
-        <v>0</v>
-      </c>
-      <c r="K40" t="n">
-        <v>0.05413101839681583</v>
-      </c>
-      <c r="L40" t="n">
-        <v>0.196351470991223</v>
-      </c>
-      <c r="M40" t="n">
-        <v>0.2326607366893173</v>
-      </c>
-      <c r="N40" t="n">
-        <v>0.9161621373991222</v>
-      </c>
-      <c r="O40" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B41" t="n">
-        <v>3</v>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>all-norm</t>
-        </is>
-      </c>
-      <c r="D41" t="n">
-        <v>0.02333375929870494</v>
-      </c>
-      <c r="E41" t="n">
-        <v>0.1122399609063723</v>
-      </c>
-      <c r="F41" t="n">
-        <v>0.1527539174578018</v>
-      </c>
-      <c r="G41" t="n">
-        <v>0.4756388355079532</v>
-      </c>
-      <c r="H41" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" t="n">
-        <v>0</v>
-      </c>
-      <c r="J41" t="n">
-        <v>0</v>
-      </c>
-      <c r="K41" t="n">
-        <v>0.04227677358919015</v>
-      </c>
-      <c r="L41" t="n">
-        <v>0.1544333887809672</v>
-      </c>
-      <c r="M41" t="n">
-        <v>0.205613164921875</v>
-      </c>
-      <c r="N41" t="n">
-        <v>0.04994741968454564</v>
-      </c>
-      <c r="O41" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B42" t="n">
-        <v>0</v>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>baseline-raw</t>
-        </is>
-      </c>
-      <c r="D42" t="n">
-        <v>0.9874637896670498</v>
-      </c>
-      <c r="E42" t="n">
-        <v>0.777102010868192</v>
-      </c>
-      <c r="F42" t="n">
-        <v>0.9937121261547782</v>
-      </c>
-      <c r="G42" t="n">
-        <v>0.4835966844994926</v>
-      </c>
-      <c r="H42" t="n">
-        <v>0</v>
-      </c>
-      <c r="I42" t="n">
-        <v>0</v>
-      </c>
-      <c r="J42" t="n">
-        <v>0</v>
-      </c>
-      <c r="K42" t="n">
-        <v>0.9413750057837428</v>
-      </c>
-      <c r="L42" t="n">
-        <v>0.7528938146576868</v>
-      </c>
-      <c r="M42" t="n">
-        <v>0.9702448174475052</v>
-      </c>
-      <c r="N42" t="n">
-        <v>0.5076992400096557</v>
-      </c>
-      <c r="O42" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B43" t="n">
-        <v>1</v>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>baseline-norm</t>
-        </is>
-      </c>
-      <c r="D43" t="n">
-        <v>0.002242688957277895</v>
-      </c>
-      <c r="E43" t="n">
-        <v>0.03810373566171948</v>
-      </c>
-      <c r="F43" t="n">
-        <v>0.04735703704073868</v>
-      </c>
-      <c r="G43" t="n">
-        <v>0.8487686156610456</v>
-      </c>
-      <c r="H43" t="n">
-        <v>0</v>
-      </c>
-      <c r="I43" t="n">
-        <v>0</v>
-      </c>
-      <c r="J43" t="n">
-        <v>0</v>
-      </c>
-      <c r="K43" t="n">
-        <v>0.01540180617310149</v>
-      </c>
-      <c r="L43" t="n">
-        <v>0.09810274962560186</v>
-      </c>
-      <c r="M43" t="n">
-        <v>0.124104013525355</v>
-      </c>
-      <c r="N43" t="n">
-        <v>-0.038590956324833</v>
-      </c>
-      <c r="O43" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B44" t="n">
-        <v>2</v>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>all-raw</t>
-        </is>
-      </c>
-      <c r="D44" t="n">
-        <v>0.0002255048174374992</v>
-      </c>
-      <c r="E44" t="n">
-        <v>0.01182776022622138</v>
-      </c>
-      <c r="F44" t="n">
-        <v>0.01501681781994771</v>
-      </c>
-      <c r="G44" t="n">
-        <v>0.9995783330966469</v>
-      </c>
-      <c r="H44" t="n">
-        <v>0</v>
-      </c>
-      <c r="I44" t="n">
-        <v>0</v>
-      </c>
-      <c r="J44" t="n">
-        <v>0</v>
-      </c>
-      <c r="K44" t="n">
-        <v>0.03589581261852858</v>
-      </c>
-      <c r="L44" t="n">
-        <v>0.1568481929912974</v>
-      </c>
-      <c r="M44" t="n">
-        <v>0.1894619028156547</v>
-      </c>
-      <c r="N44" t="n">
-        <v>0.9328791450125332</v>
-      </c>
-      <c r="O44" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B45" t="n">
-        <v>3</v>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>all-norm</t>
-        </is>
-      </c>
-      <c r="D45" t="n">
-        <v>0.01914761385981106</v>
-      </c>
-      <c r="E45" t="n">
-        <v>0.1000707694523143</v>
-      </c>
-      <c r="F45" t="n">
-        <v>0.1383749032874497</v>
-      </c>
-      <c r="G45" t="n">
-        <v>0.5172374552444661</v>
-      </c>
-      <c r="H45" t="n">
-        <v>0</v>
-      </c>
-      <c r="I45" t="n">
-        <v>0</v>
-      </c>
-      <c r="J45" t="n">
-        <v>0</v>
-      </c>
-      <c r="K45" t="n">
-        <v>0.03799129651796557</v>
-      </c>
-      <c r="L45" t="n">
-        <v>0.1456545896025763</v>
-      </c>
-      <c r="M45" t="n">
-        <v>0.1949135616573808</v>
-      </c>
-      <c r="N45" t="n">
-        <v>0.04213782877298466</v>
-      </c>
-      <c r="O45" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="R33" t="n">
+        <v>-0.22</v>
+      </c>
+      <c r="S33" t="n">
         <v>13</v>
       </c>
     </row>

</xml_diff>